<commit_message>
EPBDS-12296 EPBDS-7160 Replace *Value types with Java native types
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10351_SpreadsheetResult_CastingCells_Convertation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10351_SpreadsheetResult_CastingCells_Convertation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-10351_SpreadsheetResult_Cells_Convertation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4122CDA0-CD91-430C-BDAE-A9A065BC6C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152F2CFF-FC40-4DE4-B7FB-0D113359B0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5170" yWindow="2610" windowWidth="28800" windowHeight="15560" xr2:uid="{F1B16C8E-A7A5-4827-B739-31AC007C14E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F1B16C8E-A7A5-4827-B739-31AC007C14E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
   <si>
     <t>Environment</t>
   </si>
@@ -66,12 +66,6 @@
     <t>BigDecimal</t>
   </si>
   <si>
-    <t>BigIntegerValue</t>
-  </si>
-  <si>
-    <t>BigDecimalValue</t>
-  </si>
-  <si>
     <t>= new IntValue(1)</t>
   </si>
   <si>
@@ -87,12 +81,6 @@
     <t>= new BigDecimal(1)</t>
   </si>
   <si>
-    <t>= new BigIntegerValue(1)</t>
-  </si>
-  <si>
-    <t>= new BigDecimalValue(1)</t>
-  </si>
-  <si>
     <t>= new BigInteger("1")</t>
   </si>
   <si>
@@ -147,12 +135,6 @@
     <t>= $Calc.$Value1$BigDecimal + $Calc.$Value1$BigDecimal</t>
   </si>
   <si>
-    <t>= $Calc.$Value1$BigDecimalValue + $Calc.$Value1$BigDecimalValue</t>
-  </si>
-  <si>
-    <t>= $Calc.$Value1$BigIntegerValue + $Calc.$Value1$BigIntegerValue</t>
-  </si>
-  <si>
     <t>= sum($Calc.$ArrValue$ByteValue)</t>
   </si>
   <si>
@@ -175,12 +157,6 @@
   </si>
   <si>
     <t>= sum($Calc.$ArrValue$BigDecimal)</t>
-  </si>
-  <si>
-    <t>= sum($Calc.$ArrValue$BigDecimalValue)</t>
-  </si>
-  <si>
-    <t>= sum($Calc.$ArrValue$BigIntegerValue)</t>
   </si>
   <si>
     <t>Spreadsheet SpreadsheetResult Calc2(SpreadsheetResult calc)</t>
@@ -289,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -305,9 +281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -345,7 +321,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -451,7 +427,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -601,25 +577,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62153417-A088-4245-9B83-DF55A2AC87D7}">
-  <dimension ref="C4:F78"/>
+  <dimension ref="C4:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69:E78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.7265625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.81640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="59.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -627,532 +603,454 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C30" t="s">
+      <c r="F64" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C31" t="s">
+      <c r="D65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C32" t="s">
+      <c r="D66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C33" t="s">
+      <c r="D67" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
+      <c r="D68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C35" t="s">
+      <c r="D69" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C36" t="s">
+      <c r="D70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C37" t="s">
+      <c r="D71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C45" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C46" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C49" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C58" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C59" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C60" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C67" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C68" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" t="s">
-        <v>26</v>
-      </c>
-      <c r="E68" t="s">
-        <v>25</v>
-      </c>
-      <c r="F68" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C69" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C71" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C72" t="s">
-        <v>8</v>
-      </c>
       <c r="D72" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C73" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C74" t="s">
-        <v>10</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C75" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C76" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C77" t="s">
-        <v>13</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C78" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>